<commit_message>
edit Fav and Cart
</commit_message>
<xml_diff>
--- a/PCP/server/data/Amazon.xlsx
+++ b/PCP/server/data/Amazon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da53ec7f57a4e4a2/Desktop/homework/RIT_Classes/SWEN.732.01 - Collaborative Software Dev. (SWEN73201.2235)/Project/SWEN732-team1/PCP/server/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kayahir/Desktop/SWEN732-team1/PCP/server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{28C36BDE-75FD-439B-B090-320EFD189174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC3300B6-CE08-44C8-AE3B-1B4B304EB359}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B275ACC2-F01A-C44E-AE8D-3080E350704E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="1078">
   <si>
     <t>ProductName</t>
   </si>
@@ -3251,6 +3251,9 @@
   </si>
   <si>
     <t>https://media.wired.com/photos/64daad6b4a854832b16fd3bc/master/w_2240,c_limit/How-to-Choose-a-Laptop-August-2023-Gear.jpg</t>
+  </si>
+  <si>
+    <t>https://media.wired.com/photos/5b22c5c4b878a15e9ce80d92/master/w_2240,c_limit/iphonex-TA.jpg</t>
   </si>
 </sst>
 </file>
@@ -3638,12 +3641,12 @@
   <dimension ref="A1:I331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F340" sqref="F340"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3672,7 +3675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3685,8 +3688,8 @@
       <c r="D2" t="s">
         <v>669</v>
       </c>
-      <c r="E2" t="s">
-        <v>1076</v>
+      <c r="E2" s="2" t="s">
+        <v>1077</v>
       </c>
       <c r="F2" t="s">
         <v>673</v>
@@ -3701,7 +3704,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3846,7 +3849,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3904,7 +3907,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3991,7 +3994,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4020,7 +4023,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -4049,7 +4052,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4107,7 +4110,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -4136,7 +4139,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -4165,7 +4168,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -4194,7 +4197,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -4223,7 +4226,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -4252,7 +4255,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -4310,7 +4313,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -4339,7 +4342,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -4368,7 +4371,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -4426,7 +4429,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4455,7 +4458,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -4513,7 +4516,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -4542,7 +4545,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4571,7 +4574,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4600,7 +4603,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4629,7 +4632,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -4658,7 +4661,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -4687,7 +4690,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -4716,7 +4719,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -4745,7 +4748,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -4774,7 +4777,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -4803,7 +4806,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -4832,7 +4835,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -4890,7 +4893,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -4919,7 +4922,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -4948,7 +4951,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -4977,7 +4980,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -5006,7 +5009,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -5035,7 +5038,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -5064,7 +5067,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -5122,7 +5125,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -5151,7 +5154,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -5180,7 +5183,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -5209,7 +5212,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -5267,7 +5270,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -5296,7 +5299,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -5354,7 +5357,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -5383,7 +5386,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -5441,7 +5444,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -5470,7 +5473,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -5499,7 +5502,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -5528,7 +5531,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -5586,7 +5589,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -5615,7 +5618,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -5644,7 +5647,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -5673,7 +5676,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -5702,7 +5705,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -5731,7 +5734,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -5760,7 +5763,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -5789,7 +5792,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -5818,7 +5821,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -5847,7 +5850,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -5876,7 +5879,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -5905,7 +5908,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -5934,7 +5937,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -5963,7 +5966,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -6021,7 +6024,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -6050,7 +6053,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -6079,7 +6082,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -6108,7 +6111,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -6137,7 +6140,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -6166,7 +6169,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -6195,7 +6198,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -6224,7 +6227,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -6253,7 +6256,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -6282,7 +6285,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -6311,7 +6314,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -6340,7 +6343,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -6369,7 +6372,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -6427,7 +6430,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -6456,7 +6459,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -6485,7 +6488,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -6514,7 +6517,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -6543,7 +6546,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -6572,7 +6575,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -6601,7 +6604,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -6630,7 +6633,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -6659,7 +6662,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -6688,7 +6691,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -6717,7 +6720,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -6746,7 +6749,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -6775,7 +6778,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -6804,7 +6807,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -6833,7 +6836,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -6862,7 +6865,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -6920,7 +6923,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -6949,7 +6952,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -6978,7 +6981,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -7007,7 +7010,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -7065,7 +7068,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -7094,7 +7097,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -7152,7 +7155,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -7181,7 +7184,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -7210,7 +7213,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -7239,7 +7242,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -7268,7 +7271,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -7297,7 +7300,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -7326,7 +7329,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -7355,7 +7358,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -7384,7 +7387,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -7413,7 +7416,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -7442,7 +7445,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -7471,7 +7474,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -7500,7 +7503,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -7529,7 +7532,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -7558,7 +7561,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -7587,7 +7590,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -7616,7 +7619,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -7645,7 +7648,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -7674,7 +7677,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -7703,7 +7706,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -7732,7 +7735,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -7761,7 +7764,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -7790,7 +7793,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -7819,7 +7822,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -7848,7 +7851,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -7877,7 +7880,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -7906,7 +7909,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -7935,7 +7938,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -7964,7 +7967,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -7993,7 +7996,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -8022,7 +8025,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -8080,7 +8083,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -8109,7 +8112,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -8138,7 +8141,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -8167,7 +8170,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -8196,7 +8199,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>165</v>
       </c>
@@ -8225,7 +8228,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>166</v>
       </c>
@@ -8254,7 +8257,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -8283,7 +8286,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -8312,7 +8315,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>169</v>
       </c>
@@ -8341,7 +8344,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>170</v>
       </c>
@@ -8370,7 +8373,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>171</v>
       </c>
@@ -8399,7 +8402,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -8428,7 +8431,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -8457,7 +8460,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>174</v>
       </c>
@@ -8486,7 +8489,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -8515,7 +8518,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -8544,7 +8547,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>177</v>
       </c>
@@ -8573,7 +8576,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>178</v>
       </c>
@@ -8602,7 +8605,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>179</v>
       </c>
@@ -8631,7 +8634,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -8660,7 +8663,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -8689,7 +8692,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -8718,7 +8721,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>183</v>
       </c>
@@ -8747,7 +8750,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>184</v>
       </c>
@@ -8776,7 +8779,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -8805,7 +8808,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -8834,7 +8837,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>187</v>
       </c>
@@ -8863,7 +8866,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -8892,7 +8895,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>189</v>
       </c>
@@ -8921,7 +8924,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>190</v>
       </c>
@@ -8950,7 +8953,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -8979,7 +8982,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>192</v>
       </c>
@@ -9008,7 +9011,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>193</v>
       </c>
@@ -9037,7 +9040,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -9066,7 +9069,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>195</v>
       </c>
@@ -9095,7 +9098,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>196</v>
       </c>
@@ -9124,7 +9127,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -9153,7 +9156,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>198</v>
       </c>
@@ -9182,7 +9185,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -9211,7 +9214,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -9240,7 +9243,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>201</v>
       </c>
@@ -9269,7 +9272,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>202</v>
       </c>
@@ -9298,7 +9301,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>203</v>
       </c>
@@ -9327,7 +9330,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>204</v>
       </c>
@@ -9356,7 +9359,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>205</v>
       </c>
@@ -9385,7 +9388,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>206</v>
       </c>
@@ -9414,7 +9417,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>207</v>
       </c>
@@ -9443,7 +9446,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>208</v>
       </c>
@@ -9472,7 +9475,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -9501,7 +9504,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>210</v>
       </c>
@@ -9530,7 +9533,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>211</v>
       </c>
@@ -9559,7 +9562,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -9588,7 +9591,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>213</v>
       </c>
@@ -9617,7 +9620,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>214</v>
       </c>
@@ -9646,7 +9649,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>215</v>
       </c>
@@ -9675,7 +9678,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>216</v>
       </c>
@@ -9704,7 +9707,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>217</v>
       </c>
@@ -9733,7 +9736,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -9762,7 +9765,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>219</v>
       </c>
@@ -9791,7 +9794,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>220</v>
       </c>
@@ -9820,7 +9823,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>221</v>
       </c>
@@ -9849,7 +9852,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>222</v>
       </c>
@@ -9878,7 +9881,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>223</v>
       </c>
@@ -9907,7 +9910,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>224</v>
       </c>
@@ -9936,7 +9939,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>225</v>
       </c>
@@ -9965,7 +9968,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>226</v>
       </c>
@@ -9994,7 +9997,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>227</v>
       </c>
@@ -10023,7 +10026,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -10052,7 +10055,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>229</v>
       </c>
@@ -10081,7 +10084,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>230</v>
       </c>
@@ -10110,7 +10113,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>231</v>
       </c>
@@ -10139,7 +10142,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>232</v>
       </c>
@@ -10168,7 +10171,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>233</v>
       </c>
@@ -10197,7 +10200,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>234</v>
       </c>
@@ -10226,7 +10229,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>235</v>
       </c>
@@ -10255,7 +10258,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>236</v>
       </c>
@@ -10284,7 +10287,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>237</v>
       </c>
@@ -10313,7 +10316,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>238</v>
       </c>
@@ -10342,7 +10345,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>239</v>
       </c>
@@ -10371,7 +10374,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>240</v>
       </c>
@@ -10400,7 +10403,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>241</v>
       </c>
@@ -10429,7 +10432,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>242</v>
       </c>
@@ -10458,7 +10461,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>243</v>
       </c>
@@ -10487,7 +10490,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>244</v>
       </c>
@@ -10516,7 +10519,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>245</v>
       </c>
@@ -10545,7 +10548,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>246</v>
       </c>
@@ -10574,7 +10577,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -10603,7 +10606,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>248</v>
       </c>
@@ -10632,7 +10635,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>249</v>
       </c>
@@ -10661,7 +10664,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>250</v>
       </c>
@@ -10690,7 +10693,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>251</v>
       </c>
@@ -10719,7 +10722,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>252</v>
       </c>
@@ -10748,7 +10751,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>253</v>
       </c>
@@ -10777,7 +10780,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>254</v>
       </c>
@@ -10806,7 +10809,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>255</v>
       </c>
@@ -10835,7 +10838,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>256</v>
       </c>
@@ -10864,7 +10867,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>257</v>
       </c>
@@ -10893,7 +10896,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>258</v>
       </c>
@@ -10922,7 +10925,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>259</v>
       </c>
@@ -10951,7 +10954,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>260</v>
       </c>
@@ -10980,7 +10983,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>261</v>
       </c>
@@ -11009,7 +11012,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>262</v>
       </c>
@@ -11038,7 +11041,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>263</v>
       </c>
@@ -11067,7 +11070,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>264</v>
       </c>
@@ -11096,7 +11099,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>265</v>
       </c>
@@ -11125,7 +11128,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>266</v>
       </c>
@@ -11154,7 +11157,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>267</v>
       </c>
@@ -11183,7 +11186,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>268</v>
       </c>
@@ -11212,7 +11215,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>269</v>
       </c>
@@ -11241,7 +11244,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>270</v>
       </c>
@@ -11270,7 +11273,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>271</v>
       </c>
@@ -11299,7 +11302,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>272</v>
       </c>
@@ -11328,7 +11331,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>273</v>
       </c>
@@ -11357,7 +11360,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>274</v>
       </c>
@@ -11386,7 +11389,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>275</v>
       </c>
@@ -11415,7 +11418,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>276</v>
       </c>
@@ -11444,7 +11447,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>277</v>
       </c>
@@ -11473,7 +11476,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>278</v>
       </c>
@@ -11502,7 +11505,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>279</v>
       </c>
@@ -11531,7 +11534,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>280</v>
       </c>
@@ -11560,7 +11563,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>281</v>
       </c>
@@ -11589,7 +11592,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>282</v>
       </c>
@@ -11618,7 +11621,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>283</v>
       </c>
@@ -11647,7 +11650,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>284</v>
       </c>
@@ -11676,7 +11679,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>285</v>
       </c>
@@ -11705,7 +11708,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>286</v>
       </c>
@@ -11734,7 +11737,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>287</v>
       </c>
@@ -11763,7 +11766,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>288</v>
       </c>
@@ -11792,7 +11795,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>289</v>
       </c>
@@ -11821,7 +11824,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>290</v>
       </c>
@@ -11850,7 +11853,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>291</v>
       </c>
@@ -11879,7 +11882,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>292</v>
       </c>
@@ -11908,7 +11911,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>293</v>
       </c>
@@ -11937,7 +11940,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>294</v>
       </c>
@@ -11966,7 +11969,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>295</v>
       </c>
@@ -11995,7 +11998,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>296</v>
       </c>
@@ -12024,7 +12027,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>297</v>
       </c>
@@ -12053,7 +12056,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>298</v>
       </c>
@@ -12082,7 +12085,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>299</v>
       </c>
@@ -12111,7 +12114,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>300</v>
       </c>
@@ -12140,7 +12143,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>301</v>
       </c>
@@ -12169,7 +12172,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>302</v>
       </c>
@@ -12198,7 +12201,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>303</v>
       </c>
@@ -12227,7 +12230,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>304</v>
       </c>
@@ -12256,7 +12259,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>305</v>
       </c>
@@ -12285,7 +12288,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>306</v>
       </c>
@@ -12314,7 +12317,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>307</v>
       </c>
@@ -12343,7 +12346,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>308</v>
       </c>
@@ -12372,7 +12375,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>309</v>
       </c>
@@ -12401,7 +12404,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>310</v>
       </c>
@@ -12430,7 +12433,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>311</v>
       </c>
@@ -12459,7 +12462,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>312</v>
       </c>
@@ -12488,7 +12491,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>313</v>
       </c>
@@ -12517,7 +12520,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>314</v>
       </c>
@@ -12546,7 +12549,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>315</v>
       </c>
@@ -12575,7 +12578,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>316</v>
       </c>
@@ -12604,7 +12607,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>317</v>
       </c>
@@ -12633,7 +12636,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>318</v>
       </c>
@@ -12662,7 +12665,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>319</v>
       </c>
@@ -12691,7 +12694,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>320</v>
       </c>
@@ -12720,7 +12723,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>321</v>
       </c>
@@ -12749,7 +12752,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>322</v>
       </c>
@@ -12778,7 +12781,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>323</v>
       </c>
@@ -12807,7 +12810,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>324</v>
       </c>
@@ -12836,7 +12839,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>325</v>
       </c>
@@ -12865,7 +12868,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>326</v>
       </c>
@@ -12894,7 +12897,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>327</v>
       </c>
@@ -12923,7 +12926,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>328</v>
       </c>
@@ -12952,7 +12955,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>329</v>
       </c>
@@ -12981,7 +12984,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>330</v>
       </c>
@@ -13010,7 +13013,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>331</v>
       </c>
@@ -13039,7 +13042,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>332</v>
       </c>
@@ -13068,7 +13071,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>333</v>
       </c>
@@ -13097,7 +13100,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>334</v>
       </c>
@@ -13126,7 +13129,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>335</v>
       </c>
@@ -13155,7 +13158,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>336</v>
       </c>
@@ -13184,7 +13187,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>337</v>
       </c>
@@ -13213,7 +13216,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>338</v>
       </c>
@@ -13574,6 +13577,7 @@
     <hyperlink ref="B329" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
     <hyperlink ref="B330" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
     <hyperlink ref="B331" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="E2" r:id="rId331" xr:uid="{D2AF21EA-3A7D-DD4B-BECE-7DDCA338BE1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>